<commit_message>
remove nearZeroVar cols before lr
</commit_message>
<xml_diff>
--- a/data/Species Taxonomy Marked.xlsx
+++ b/data/Species Taxonomy Marked.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAGAVENDRA KUMAR R\OneDrive\Documents\CSCI-GA.2565-001 - Machine Learning\crc-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E3586A4E-A127-4734-A3D2-AB6B4FBD487C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363EE883-9BAA-4ABB-8748-AFB664811C78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="6108" yWindow="2076" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Species Taxonomy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Species Taxonomy'!$A$1:$A$1941</definedName>
+  </definedNames>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -17494,7 +17497,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -17972,9 +17975,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -18329,11 +18333,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1941"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1814" workbookViewId="0">
-      <selection activeCell="B1829" sqref="B1829"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18651,13 +18655,13 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>86</v>
       </c>
     </row>
@@ -24272,13 +24276,13 @@
       </c>
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A540" t="s">
+      <c r="A540" s="2" t="s">
         <v>1617</v>
       </c>
-      <c r="B540" t="s">
+      <c r="B540" s="2" t="s">
         <v>1618</v>
       </c>
-      <c r="C540" t="s">
+      <c r="C540" s="2" t="s">
         <v>1619</v>
       </c>
     </row>
@@ -25504,13 +25508,13 @@
       </c>
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A652" t="s">
+      <c r="A652" s="2" t="s">
         <v>1953</v>
       </c>
-      <c r="B652" t="s">
+      <c r="B652" s="2" t="s">
         <v>1954</v>
       </c>
-      <c r="C652" t="s">
+      <c r="C652" s="2" t="s">
         <v>1955</v>
       </c>
     </row>
@@ -26395,13 +26399,13 @@
       </c>
     </row>
     <row r="733" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A733" t="s">
+      <c r="A733" s="2" t="s">
         <v>2196</v>
       </c>
-      <c r="B733" t="s">
+      <c r="B733" s="2" t="s">
         <v>2197</v>
       </c>
-      <c r="C733" t="s">
+      <c r="C733" s="2" t="s">
         <v>2198</v>
       </c>
     </row>
@@ -26692,13 +26696,13 @@
       </c>
     </row>
     <row r="760" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A760" t="s">
+      <c r="A760" s="2" t="s">
         <v>2277</v>
       </c>
-      <c r="B760" t="s">
+      <c r="B760" s="2" t="s">
         <v>2278</v>
       </c>
-      <c r="C760" t="s">
+      <c r="C760" s="2" t="s">
         <v>2279</v>
       </c>
     </row>
@@ -26736,13 +26740,13 @@
       </c>
     </row>
     <row r="764" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A764" t="s">
+      <c r="A764" s="2" t="s">
         <v>2289</v>
       </c>
-      <c r="B764" t="s">
+      <c r="B764" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="C764" t="s">
+      <c r="C764" s="2" t="s">
         <v>2291</v>
       </c>
     </row>
@@ -26791,13 +26795,13 @@
       </c>
     </row>
     <row r="769" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A769" t="s">
+      <c r="A769" s="2" t="s">
         <v>2304</v>
       </c>
-      <c r="B769" t="s">
+      <c r="B769" s="2" t="s">
         <v>2305</v>
       </c>
-      <c r="C769" t="s">
+      <c r="C769" s="2" t="s">
         <v>2306</v>
       </c>
     </row>
@@ -27143,13 +27147,13 @@
       </c>
     </row>
     <row r="801" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A801" t="s">
+      <c r="A801" s="2" t="s">
         <v>2400</v>
       </c>
-      <c r="B801" t="s">
+      <c r="B801" s="2" t="s">
         <v>2401</v>
       </c>
-      <c r="C801" t="s">
+      <c r="C801" s="2" t="s">
         <v>2402</v>
       </c>
     </row>
@@ -28694,13 +28698,13 @@
       </c>
     </row>
     <row r="942" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A942" t="s">
+      <c r="A942" s="2" t="s">
         <v>2823</v>
       </c>
-      <c r="B942" t="s">
+      <c r="B942" s="2" t="s">
         <v>2824</v>
       </c>
-      <c r="C942" t="s">
+      <c r="C942" s="2" t="s">
         <v>2825</v>
       </c>
     </row>
@@ -30234,13 +30238,13 @@
       </c>
     </row>
     <row r="1082" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1082" t="s">
+      <c r="A1082" s="2" t="s">
         <v>3243</v>
       </c>
-      <c r="B1082" t="s">
+      <c r="B1082" s="2" t="s">
         <v>3244</v>
       </c>
-      <c r="C1082" t="s">
+      <c r="C1082" s="2" t="s">
         <v>3245</v>
       </c>
     </row>
@@ -33380,13 +33384,13 @@
       </c>
     </row>
     <row r="1368" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1368" t="s">
+      <c r="A1368" s="2" t="s">
         <v>4101</v>
       </c>
-      <c r="B1368" t="s">
+      <c r="B1368" s="2" t="s">
         <v>4102</v>
       </c>
-      <c r="C1368" t="s">
+      <c r="C1368" s="2" t="s">
         <v>4103</v>
       </c>
     </row>
@@ -33457,13 +33461,13 @@
       </c>
     </row>
     <row r="1375" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1375" t="s">
+      <c r="A1375" s="2" t="s">
         <v>4122</v>
       </c>
-      <c r="B1375" t="s">
+      <c r="B1375" s="2" t="s">
         <v>4123</v>
       </c>
-      <c r="C1375" t="s">
+      <c r="C1375" s="2" t="s">
         <v>4124</v>
       </c>
     </row>
@@ -36724,13 +36728,13 @@
       </c>
     </row>
     <row r="1672" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1672" t="s">
+      <c r="A1672" s="2" t="s">
         <v>5013</v>
       </c>
-      <c r="B1672" t="s">
+      <c r="B1672" s="2" t="s">
         <v>5014</v>
       </c>
-      <c r="C1672" t="s">
+      <c r="C1672" s="2" t="s">
         <v>5015</v>
       </c>
     </row>
@@ -38671,13 +38675,13 @@
       </c>
     </row>
     <row r="1849" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1849" t="s">
+      <c r="A1849" s="2" t="s">
         <v>5544</v>
       </c>
-      <c r="B1849" t="s">
+      <c r="B1849" s="2" t="s">
         <v>5545</v>
       </c>
-      <c r="C1849" t="s">
+      <c r="C1849" s="2" t="s">
         <v>5546</v>
       </c>
     </row>
@@ -38759,13 +38763,13 @@
       </c>
     </row>
     <row r="1857" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1857" t="s">
+      <c r="A1857" s="2" t="s">
         <v>5568</v>
       </c>
-      <c r="B1857" t="s">
+      <c r="B1857" s="2" t="s">
         <v>5569</v>
       </c>
-      <c r="C1857" t="s">
+      <c r="C1857" s="2" t="s">
         <v>5570</v>
       </c>
     </row>
@@ -38891,13 +38895,13 @@
       </c>
     </row>
     <row r="1869" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1869" t="s">
+      <c r="A1869" s="2" t="s">
         <v>5604</v>
       </c>
-      <c r="B1869" t="s">
+      <c r="B1869" s="2" t="s">
         <v>5605</v>
       </c>
-      <c r="C1869" t="s">
+      <c r="C1869" s="2" t="s">
         <v>5606</v>
       </c>
     </row>
@@ -38913,13 +38917,13 @@
       </c>
     </row>
     <row r="1871" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1871" t="s">
+      <c r="A1871" s="2" t="s">
         <v>5610</v>
       </c>
-      <c r="B1871" t="s">
+      <c r="B1871" s="2" t="s">
         <v>5611</v>
       </c>
-      <c r="C1871" t="s">
+      <c r="C1871" s="2" t="s">
         <v>5612</v>
       </c>
     </row>
@@ -39243,13 +39247,13 @@
       </c>
     </row>
     <row r="1901" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1901" t="s">
+      <c r="A1901" s="2" t="s">
         <v>5700</v>
       </c>
-      <c r="B1901" t="s">
+      <c r="B1901" s="2" t="s">
         <v>5701</v>
       </c>
-      <c r="C1901" t="s">
+      <c r="C1901" s="2" t="s">
         <v>5702</v>
       </c>
     </row>
@@ -39353,13 +39357,13 @@
       </c>
     </row>
     <row r="1911" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1911" t="s">
+      <c r="A1911" s="2" t="s">
         <v>5730</v>
       </c>
-      <c r="B1911" t="s">
+      <c r="B1911" s="2" t="s">
         <v>5731</v>
       </c>
-      <c r="C1911" t="s">
+      <c r="C1911" s="2" t="s">
         <v>5732</v>
       </c>
     </row>
@@ -39650,13 +39654,13 @@
       </c>
     </row>
     <row r="1938" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1938" t="s">
+      <c r="A1938" s="2" t="s">
         <v>5811</v>
       </c>
-      <c r="B1938" t="s">
+      <c r="B1938" s="2" t="s">
         <v>5812</v>
       </c>
-      <c r="C1938" t="s">
+      <c r="C1938" s="2" t="s">
         <v>5813</v>
       </c>
     </row>

</xml_diff>